<commit_message>
June 2 Updated version
</commit_message>
<xml_diff>
--- a/Data_RLA/summary.xlsx
+++ b/Data_RLA/summary.xlsx
@@ -468,28 +468,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="C4">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="D4">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="E4">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -497,28 +497,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="C5">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="D5">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F5">
+        <v>47</v>
+      </c>
+      <c r="G5">
         <v>25</v>
       </c>
-      <c r="G5">
-        <v>19</v>
-      </c>
       <c r="H5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -526,28 +526,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E6">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="F6">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="G6">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="H6">
+        <v>46</v>
+      </c>
+      <c r="I6">
         <v>32</v>
-      </c>
-      <c r="I6">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -555,28 +555,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="F7">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="G7">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="H7">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="I7">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -584,25 +584,25 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="F8">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="G8">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H8">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <v>22</v>
@@ -613,28 +613,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="C9">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="D9">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="F9">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -701,28 +701,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>406382</v>
+        <v>300436</v>
       </c>
       <c r="C4">
-        <v>373786</v>
+        <v>314778</v>
       </c>
       <c r="D4">
-        <v>336690</v>
+        <v>315289</v>
       </c>
       <c r="E4">
-        <v>297533</v>
+        <v>311102</v>
       </c>
       <c r="F4">
-        <v>24450</v>
+        <v>126782</v>
       </c>
       <c r="G4">
-        <v>17517</v>
+        <v>128252</v>
       </c>
       <c r="H4">
-        <v>18527</v>
+        <v>123818</v>
       </c>
       <c r="I4">
-        <v>11963</v>
+        <v>116505</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -730,28 +730,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>392862</v>
+        <v>307688</v>
       </c>
       <c r="C5">
-        <v>351466</v>
+        <v>316621</v>
       </c>
       <c r="D5">
-        <v>327108</v>
+        <v>314001</v>
       </c>
       <c r="E5">
-        <v>282754</v>
+        <v>307137</v>
       </c>
       <c r="F5">
-        <v>49952</v>
+        <v>231587</v>
       </c>
       <c r="G5">
-        <v>43398</v>
+        <v>231458</v>
       </c>
       <c r="H5">
-        <v>36360</v>
+        <v>220707</v>
       </c>
       <c r="I5">
-        <v>32298</v>
+        <v>205795</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -759,28 +759,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>280198</v>
+        <v>251093</v>
       </c>
       <c r="C6">
-        <v>254716</v>
+        <v>241932</v>
       </c>
       <c r="D6">
-        <v>235757</v>
+        <v>232006</v>
       </c>
       <c r="E6">
-        <v>210994</v>
+        <v>221293</v>
       </c>
       <c r="F6">
-        <v>541038</v>
+        <v>600290</v>
       </c>
       <c r="G6">
-        <v>454191</v>
+        <v>578086</v>
       </c>
       <c r="H6">
-        <v>379971</v>
+        <v>543163</v>
       </c>
       <c r="I6">
-        <v>338796</v>
+        <v>503740</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -788,28 +788,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>126336</v>
+        <v>110353</v>
       </c>
       <c r="C7">
-        <v>113762</v>
+        <v>107725</v>
       </c>
       <c r="D7">
-        <v>103488</v>
+        <v>103444</v>
       </c>
       <c r="E7">
-        <v>93401</v>
+        <v>98883</v>
       </c>
       <c r="F7">
-        <v>237985</v>
+        <v>233124</v>
       </c>
       <c r="G7">
-        <v>199066</v>
+        <v>225425</v>
       </c>
       <c r="H7">
-        <v>172416</v>
+        <v>212182</v>
       </c>
       <c r="I7">
-        <v>144050</v>
+        <v>196800</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -817,28 +817,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>56378</v>
+        <v>47042</v>
       </c>
       <c r="C8">
-        <v>50418</v>
+        <v>46680</v>
       </c>
       <c r="D8">
-        <v>46152</v>
+        <v>45388</v>
       </c>
       <c r="E8">
-        <v>42399</v>
+        <v>43677</v>
       </c>
       <c r="F8">
-        <v>47981</v>
+        <v>72565</v>
       </c>
       <c r="G8">
-        <v>41562</v>
+        <v>71051</v>
       </c>
       <c r="H8">
-        <v>35963</v>
+        <v>67158</v>
       </c>
       <c r="I8">
-        <v>30440</v>
+        <v>62595</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -846,28 +846,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>27673902</v>
+        <v>20279439</v>
       </c>
       <c r="C9">
-        <v>24602292</v>
+        <v>21391712</v>
       </c>
       <c r="D9">
-        <v>22121167</v>
+        <v>21566370</v>
       </c>
       <c r="E9">
-        <v>20568259</v>
+        <v>21215148</v>
       </c>
       <c r="F9">
-        <v>1419445</v>
+        <v>6021139</v>
       </c>
       <c r="G9">
-        <v>1158908</v>
+        <v>6105327</v>
       </c>
       <c r="H9">
-        <v>866781</v>
+        <v>5849526</v>
       </c>
       <c r="I9">
-        <v>873896</v>
+        <v>5509857</v>
       </c>
     </row>
   </sheetData>
@@ -934,28 +934,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>95469</v>
+        <v>113527</v>
       </c>
       <c r="C4">
-        <v>81482</v>
+        <v>114376</v>
       </c>
       <c r="D4">
-        <v>69974</v>
+        <v>110529</v>
       </c>
       <c r="E4">
-        <v>60290</v>
+        <v>104431</v>
       </c>
       <c r="F4">
-        <v>4244</v>
+        <v>49118</v>
       </c>
       <c r="G4">
-        <v>3354</v>
+        <v>47671</v>
       </c>
       <c r="H4">
-        <v>2461</v>
+        <v>44008</v>
       </c>
       <c r="I4">
-        <v>1070</v>
+        <v>39615</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -963,28 +963,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>88713</v>
+        <v>114071</v>
       </c>
       <c r="C5">
-        <v>74531</v>
+        <v>112248</v>
       </c>
       <c r="D5">
-        <v>64583</v>
+        <v>106862</v>
       </c>
       <c r="E5">
-        <v>56204</v>
+        <v>100500</v>
       </c>
       <c r="F5">
-        <v>9785</v>
+        <v>88368</v>
       </c>
       <c r="G5">
-        <v>7271</v>
+        <v>84585</v>
       </c>
       <c r="H5">
-        <v>5250</v>
+        <v>77317</v>
       </c>
       <c r="I5">
-        <v>4184</v>
+        <v>69107</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -992,28 +992,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>59423</v>
+        <v>85795</v>
       </c>
       <c r="C6">
-        <v>51375</v>
+        <v>79888</v>
       </c>
       <c r="D6">
-        <v>44974</v>
+        <v>73790</v>
       </c>
       <c r="E6">
-        <v>37729</v>
+        <v>68593</v>
       </c>
       <c r="F6">
-        <v>98848</v>
+        <v>218317</v>
       </c>
       <c r="G6">
-        <v>76923</v>
+        <v>201961</v>
       </c>
       <c r="H6">
-        <v>60647</v>
+        <v>182266</v>
       </c>
       <c r="I6">
-        <v>49002</v>
+        <v>162480</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1021,28 +1021,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>27462</v>
+        <v>38741</v>
       </c>
       <c r="C7">
-        <v>23454</v>
+        <v>36323</v>
       </c>
       <c r="D7">
-        <v>20202</v>
+        <v>33565</v>
       </c>
       <c r="E7">
-        <v>17752</v>
+        <v>31038</v>
       </c>
       <c r="F7">
-        <v>44261</v>
+        <v>86564</v>
       </c>
       <c r="G7">
-        <v>34524</v>
+        <v>80354</v>
       </c>
       <c r="H7">
-        <v>27849</v>
+        <v>72642</v>
       </c>
       <c r="I7">
-        <v>22420</v>
+        <v>64923</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1050,28 +1050,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>12794</v>
+        <v>16982</v>
       </c>
       <c r="C8">
-        <v>11013</v>
+        <v>16174</v>
       </c>
       <c r="D8">
-        <v>9292</v>
+        <v>15189</v>
       </c>
       <c r="E8">
-        <v>8050</v>
+        <v>14097</v>
       </c>
       <c r="F8">
-        <v>9207</v>
+        <v>27352</v>
       </c>
       <c r="G8">
-        <v>7017</v>
+        <v>25655</v>
       </c>
       <c r="H8">
-        <v>5752</v>
+        <v>23272</v>
       </c>
       <c r="I8">
-        <v>4604</v>
+        <v>20867</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1079,28 +1079,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>5854068</v>
+        <v>7126521</v>
       </c>
       <c r="C9">
-        <v>4899798</v>
+        <v>7239374</v>
       </c>
       <c r="D9">
-        <v>4161626</v>
+        <v>7031779</v>
       </c>
       <c r="E9">
-        <v>3520029</v>
+        <v>6649480</v>
       </c>
       <c r="F9">
-        <v>186225</v>
+        <v>2151944</v>
       </c>
       <c r="G9">
-        <v>183391</v>
+        <v>2101272</v>
       </c>
       <c r="H9">
-        <v>152036</v>
+        <v>1940359</v>
       </c>
       <c r="I9">
-        <v>84221</v>
+        <v>1747854</v>
       </c>
     </row>
   </sheetData>
@@ -1167,28 +1167,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6201</v>
+        <v>6107</v>
       </c>
       <c r="C4">
-        <v>5258</v>
+        <v>6189</v>
       </c>
       <c r="D4">
-        <v>4491</v>
+        <v>6015</v>
       </c>
       <c r="E4">
-        <v>3897</v>
+        <v>5731</v>
       </c>
       <c r="F4">
-        <v>298</v>
+        <v>2664</v>
       </c>
       <c r="G4">
-        <v>232</v>
+        <v>2601</v>
       </c>
       <c r="H4">
-        <v>177</v>
+        <v>2416</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1196,28 +1196,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>5113</v>
+        <v>5868</v>
       </c>
       <c r="C5">
-        <v>4363</v>
+        <v>5789</v>
       </c>
       <c r="D5">
-        <v>3633</v>
+        <v>5542</v>
       </c>
       <c r="E5">
-        <v>2985</v>
+        <v>5203</v>
       </c>
       <c r="F5">
-        <v>573</v>
+        <v>4570</v>
       </c>
       <c r="G5">
-        <v>423</v>
+        <v>4383</v>
       </c>
       <c r="H5">
-        <v>351</v>
+        <v>4015</v>
       </c>
       <c r="I5">
-        <v>280</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1225,28 +1225,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>3690</v>
+        <v>4646</v>
       </c>
       <c r="C6">
-        <v>3094</v>
+        <v>4386</v>
       </c>
       <c r="D6">
-        <v>2678</v>
+        <v>4112</v>
       </c>
       <c r="E6">
-        <v>2311</v>
+        <v>3815</v>
       </c>
       <c r="F6">
-        <v>6404</v>
+        <v>11722</v>
       </c>
       <c r="G6">
-        <v>4924</v>
+        <v>10919</v>
       </c>
       <c r="H6">
-        <v>3927</v>
+        <v>9935</v>
       </c>
       <c r="I6">
-        <v>3102</v>
+        <v>8975</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1254,28 +1254,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1772</v>
+        <v>2129</v>
       </c>
       <c r="C7">
-        <v>1509</v>
+        <v>2013</v>
       </c>
       <c r="D7">
-        <v>1289</v>
+        <v>1892</v>
       </c>
       <c r="E7">
-        <v>1130</v>
+        <v>1774</v>
       </c>
       <c r="F7">
-        <v>2943</v>
+        <v>4723</v>
       </c>
       <c r="G7">
-        <v>2284</v>
+        <v>4426</v>
       </c>
       <c r="H7">
-        <v>1841</v>
+        <v>4043</v>
       </c>
       <c r="I7">
-        <v>1488</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1283,28 +1283,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>826</v>
+        <v>924</v>
       </c>
       <c r="C8">
-        <v>706</v>
+        <v>889</v>
       </c>
       <c r="D8">
-        <v>591</v>
+        <v>839</v>
       </c>
       <c r="E8">
-        <v>510</v>
+        <v>789</v>
       </c>
       <c r="F8">
-        <v>616</v>
+        <v>1489</v>
       </c>
       <c r="G8">
-        <v>468</v>
+        <v>1410</v>
       </c>
       <c r="H8">
-        <v>384</v>
+        <v>1293</v>
       </c>
       <c r="I8">
-        <v>302</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1312,28 +1312,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>367033</v>
+        <v>376072</v>
       </c>
       <c r="C9">
-        <v>304784</v>
+        <v>384129</v>
       </c>
       <c r="D9">
-        <v>257205</v>
+        <v>374545</v>
       </c>
       <c r="E9">
-        <v>215280</v>
+        <v>358667</v>
       </c>
       <c r="F9">
-        <v>15244</v>
+        <v>114511</v>
       </c>
       <c r="G9">
-        <v>11829</v>
+        <v>112368</v>
       </c>
       <c r="H9">
-        <v>11189</v>
+        <v>105102</v>
       </c>
       <c r="I9">
-        <v>7920</v>
+        <v>95295</v>
       </c>
     </row>
   </sheetData>
@@ -1400,28 +1400,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2240</v>
+        <v>2667</v>
       </c>
       <c r="C4">
-        <v>1926</v>
+        <v>2684</v>
       </c>
       <c r="D4">
-        <v>1635</v>
+        <v>2589</v>
       </c>
       <c r="E4">
-        <v>1403</v>
+        <v>2443</v>
       </c>
       <c r="F4">
-        <v>99</v>
+        <v>1151</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>1121</v>
       </c>
       <c r="H4">
-        <v>46</v>
+        <v>1031</v>
       </c>
       <c r="I4">
-        <v>62</v>
+        <v>931</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1429,28 +1429,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>2063</v>
+        <v>2681</v>
       </c>
       <c r="C5">
-        <v>1795</v>
+        <v>2639</v>
       </c>
       <c r="D5">
-        <v>1519</v>
+        <v>2514</v>
       </c>
       <c r="E5">
-        <v>1282</v>
+        <v>2350</v>
       </c>
       <c r="F5">
-        <v>209</v>
+        <v>2074</v>
       </c>
       <c r="G5">
-        <v>150</v>
+        <v>1984</v>
       </c>
       <c r="H5">
-        <v>130</v>
+        <v>1812</v>
       </c>
       <c r="I5">
-        <v>104</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1458,28 +1458,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1415</v>
+        <v>2011</v>
       </c>
       <c r="C6">
-        <v>1216</v>
+        <v>1885</v>
       </c>
       <c r="D6">
-        <v>1018</v>
+        <v>1746</v>
       </c>
       <c r="E6">
-        <v>897</v>
+        <v>1602</v>
       </c>
       <c r="F6">
-        <v>2300</v>
+        <v>5122</v>
       </c>
       <c r="G6">
-        <v>1794</v>
+        <v>4732</v>
       </c>
       <c r="H6">
-        <v>1439</v>
+        <v>4268</v>
       </c>
       <c r="I6">
-        <v>1164</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1487,28 +1487,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>637</v>
+        <v>906</v>
       </c>
       <c r="C7">
-        <v>558</v>
+        <v>851</v>
       </c>
       <c r="D7">
-        <v>486</v>
+        <v>793</v>
       </c>
       <c r="E7">
-        <v>407</v>
+        <v>733</v>
       </c>
       <c r="F7">
-        <v>1034</v>
+        <v>2031</v>
       </c>
       <c r="G7">
-        <v>808</v>
+        <v>1885</v>
       </c>
       <c r="H7">
-        <v>634</v>
+        <v>1701</v>
       </c>
       <c r="I7">
-        <v>521</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1516,28 +1516,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>301</v>
+        <v>398</v>
       </c>
       <c r="C8">
-        <v>257</v>
+        <v>380</v>
       </c>
       <c r="D8">
-        <v>224</v>
+        <v>355</v>
       </c>
       <c r="E8">
-        <v>193</v>
+        <v>330</v>
       </c>
       <c r="F8">
-        <v>215</v>
+        <v>642</v>
       </c>
       <c r="G8">
-        <v>169</v>
+        <v>602</v>
       </c>
       <c r="H8">
-        <v>129</v>
+        <v>547</v>
       </c>
       <c r="I8">
-        <v>105</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1545,28 +1545,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>135897</v>
+        <v>167136</v>
       </c>
       <c r="C9">
-        <v>115246</v>
+        <v>170037</v>
       </c>
       <c r="D9">
-        <v>96042</v>
+        <v>164709</v>
       </c>
       <c r="E9">
-        <v>82736</v>
+        <v>156344</v>
       </c>
       <c r="F9">
-        <v>6069</v>
+        <v>50558</v>
       </c>
       <c r="G9">
-        <v>3645</v>
+        <v>49359</v>
       </c>
       <c r="H9">
-        <v>2328</v>
+        <v>45492</v>
       </c>
       <c r="I9">
-        <v>3535</v>
+        <v>41045</v>
       </c>
     </row>
   </sheetData>
@@ -1633,28 +1633,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10574088</v>
+        <v>2087480</v>
       </c>
       <c r="C4">
-        <v>9112566</v>
+        <v>1655416</v>
       </c>
       <c r="D4">
-        <v>7304641</v>
+        <v>1337758</v>
       </c>
       <c r="E4">
-        <v>5538708</v>
+        <v>1095395</v>
       </c>
       <c r="F4">
-        <v>3074309</v>
+        <v>1097464</v>
       </c>
       <c r="G4">
-        <v>4589801</v>
+        <v>734073</v>
       </c>
       <c r="H4">
-        <v>5825544</v>
+        <v>540706</v>
       </c>
       <c r="I4">
-        <v>6037332</v>
+        <v>408514</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1662,28 +1662,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>7890873</v>
+        <v>1907856</v>
       </c>
       <c r="C5">
-        <v>6276321</v>
+        <v>1516774</v>
       </c>
       <c r="D5">
-        <v>4736516</v>
+        <v>1223920</v>
       </c>
       <c r="E5">
-        <v>3473843</v>
+        <v>999508</v>
       </c>
       <c r="F5">
-        <v>5310221</v>
+        <v>1874498</v>
       </c>
       <c r="G5">
-        <v>7052912</v>
+        <v>1250359</v>
       </c>
       <c r="H5">
-        <v>8303634</v>
+        <v>920054</v>
       </c>
       <c r="I5">
-        <v>8559270</v>
+        <v>693322</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1691,28 +1691,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1265593</v>
+        <v>991914</v>
       </c>
       <c r="C6">
-        <v>923073</v>
+        <v>807889</v>
       </c>
       <c r="D6">
-        <v>672075</v>
+        <v>666287</v>
       </c>
       <c r="E6">
-        <v>492638</v>
+        <v>555775</v>
       </c>
       <c r="F6">
-        <v>8956787</v>
+        <v>3832770</v>
       </c>
       <c r="G6">
-        <v>9441329</v>
+        <v>2526382</v>
       </c>
       <c r="H6">
-        <v>9722660</v>
+        <v>1899549</v>
       </c>
       <c r="I6">
-        <v>9761452</v>
+        <v>1460377</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1720,28 +1720,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>540475</v>
+        <v>466365</v>
       </c>
       <c r="C7">
-        <v>393428</v>
+        <v>378593</v>
       </c>
       <c r="D7">
-        <v>286378</v>
+        <v>311423</v>
       </c>
       <c r="E7">
-        <v>210195</v>
+        <v>259241</v>
       </c>
       <c r="F7">
-        <v>3982988</v>
+        <v>1428167</v>
       </c>
       <c r="G7">
-        <v>4148428</v>
+        <v>1016191</v>
       </c>
       <c r="H7">
-        <v>4135006</v>
+        <v>762579</v>
       </c>
       <c r="I7">
-        <v>3840300</v>
+        <v>585399</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1749,28 +1749,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>471860</v>
+        <v>231340</v>
       </c>
       <c r="C8">
-        <v>346287</v>
+        <v>186498</v>
       </c>
       <c r="D8">
-        <v>251121</v>
+        <v>152441</v>
       </c>
       <c r="E8">
-        <v>182382</v>
+        <v>126139</v>
       </c>
       <c r="F8">
-        <v>1494492</v>
+        <v>528160</v>
       </c>
       <c r="G8">
-        <v>1653186</v>
+        <v>344724</v>
       </c>
       <c r="H8">
-        <v>1752970</v>
+        <v>257122</v>
       </c>
       <c r="I8">
-        <v>1781787</v>
+        <v>196384</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1778,28 +1778,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>843392578</v>
+        <v>154002774</v>
       </c>
       <c r="C9">
-        <v>797941342</v>
+        <v>114786894</v>
       </c>
       <c r="D9">
-        <v>713674898</v>
+        <v>92154516</v>
       </c>
       <c r="E9">
-        <v>601112617</v>
+        <v>75006315</v>
       </c>
       <c r="F9">
-        <v>96393365</v>
+        <v>84954520</v>
       </c>
       <c r="G9">
-        <v>161227476</v>
+        <v>35171290</v>
       </c>
       <c r="H9">
-        <v>252555962</v>
+        <v>25660765</v>
       </c>
       <c r="I9">
-        <v>358222243</v>
+        <v>19258466</v>
       </c>
     </row>
   </sheetData>
@@ -1866,28 +1866,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2728633</v>
+        <v>323594</v>
       </c>
       <c r="C4">
-        <v>2606850</v>
+        <v>268217</v>
       </c>
       <c r="D4">
-        <v>2374927</v>
+        <v>225714</v>
       </c>
       <c r="E4">
-        <v>2080185</v>
+        <v>191838</v>
       </c>
       <c r="F4">
-        <v>374451</v>
+        <v>169419</v>
       </c>
       <c r="G4">
-        <v>579879</v>
+        <v>116256</v>
       </c>
       <c r="H4">
-        <v>805837</v>
+        <v>89605</v>
       </c>
       <c r="I4">
-        <v>971172</v>
+        <v>70588</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1895,28 +1895,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>2187168</v>
+        <v>298011</v>
       </c>
       <c r="C5">
-        <v>1973116</v>
+        <v>246553</v>
       </c>
       <c r="D5">
-        <v>1709402</v>
+        <v>206151</v>
       </c>
       <c r="E5">
-        <v>1443073</v>
+        <v>173934</v>
       </c>
       <c r="F5">
-        <v>710198</v>
+        <v>289375</v>
       </c>
       <c r="G5">
-        <v>992342</v>
+        <v>196713</v>
       </c>
       <c r="H5">
-        <v>1263555</v>
+        <v>150626</v>
       </c>
       <c r="I5">
-        <v>1454683</v>
+        <v>117697</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1924,28 +1924,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>567475</v>
+        <v>169980</v>
       </c>
       <c r="C6">
-        <v>470158</v>
+        <v>143766</v>
       </c>
       <c r="D6">
-        <v>387007</v>
+        <v>122881</v>
       </c>
       <c r="E6">
-        <v>319155</v>
+        <v>106094</v>
       </c>
       <c r="F6">
-        <v>1721794</v>
+        <v>617676</v>
       </c>
       <c r="G6">
-        <v>1867537</v>
+        <v>413658</v>
       </c>
       <c r="H6">
-        <v>1976987</v>
+        <v>324458</v>
       </c>
       <c r="I6">
-        <v>2048485</v>
+        <v>259530</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1953,28 +1953,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>250611</v>
+        <v>79529</v>
       </c>
       <c r="C7">
-        <v>207708</v>
+        <v>67127</v>
       </c>
       <c r="D7">
-        <v>171177</v>
+        <v>57300</v>
       </c>
       <c r="E7">
-        <v>141449</v>
+        <v>49442</v>
       </c>
       <c r="F7">
-        <v>785893</v>
+        <v>226481</v>
       </c>
       <c r="G7">
-        <v>848172</v>
+        <v>167441</v>
       </c>
       <c r="H7">
-        <v>885368</v>
+        <v>131214</v>
       </c>
       <c r="I7">
-        <v>887006</v>
+        <v>104927</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1982,28 +1982,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>186499</v>
+        <v>38188</v>
       </c>
       <c r="C8">
-        <v>157644</v>
+        <v>32058</v>
       </c>
       <c r="D8">
-        <v>131040</v>
+        <v>27210</v>
       </c>
       <c r="E8">
-        <v>108356</v>
+        <v>23342</v>
       </c>
       <c r="F8">
-        <v>261630</v>
+        <v>84821</v>
       </c>
       <c r="G8">
-        <v>302646</v>
+        <v>56095</v>
       </c>
       <c r="H8">
-        <v>335806</v>
+        <v>43702</v>
       </c>
       <c r="I8">
-        <v>359161</v>
+        <v>34775</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2011,28 +2011,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>187858086</v>
+        <v>22704226</v>
       </c>
       <c r="C9">
-        <v>187404402</v>
+        <v>17341947</v>
       </c>
       <c r="D9">
-        <v>180538019</v>
+        <v>14557796</v>
       </c>
       <c r="E9">
-        <v>168154347</v>
+        <v>12341708</v>
       </c>
       <c r="F9">
-        <v>10672000</v>
+        <v>13577153</v>
       </c>
       <c r="G9">
-        <v>17470831</v>
+        <v>5200102</v>
       </c>
       <c r="H9">
-        <v>27657946</v>
+        <v>3979042</v>
       </c>
       <c r="I9">
-        <v>41131513</v>
+        <v>3123461</v>
       </c>
     </row>
   </sheetData>
@@ -2099,28 +2099,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>175118</v>
+        <v>16078</v>
       </c>
       <c r="C4">
-        <v>168918</v>
+        <v>13808</v>
       </c>
       <c r="D4">
-        <v>155420</v>
+        <v>12066</v>
       </c>
       <c r="E4">
-        <v>137529</v>
+        <v>10672</v>
       </c>
       <c r="F4">
-        <v>23020</v>
+        <v>8427</v>
       </c>
       <c r="G4">
-        <v>35806</v>
+        <v>6035</v>
       </c>
       <c r="H4">
-        <v>50080</v>
+        <v>4864</v>
       </c>
       <c r="I4">
-        <v>60890</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2128,28 +2128,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>126254</v>
+        <v>14215</v>
       </c>
       <c r="C5">
-        <v>113018</v>
+        <v>12117</v>
       </c>
       <c r="D5">
-        <v>97167</v>
+        <v>10460</v>
       </c>
       <c r="E5">
-        <v>81454</v>
+        <v>9131</v>
       </c>
       <c r="F5">
-        <v>42985</v>
+        <v>13678</v>
       </c>
       <c r="G5">
-        <v>59792</v>
+        <v>9621</v>
       </c>
       <c r="H5">
-        <v>75707</v>
+        <v>7635</v>
       </c>
       <c r="I5">
-        <v>86582</v>
+        <v>6197</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2157,28 +2157,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>35576</v>
+        <v>9181</v>
       </c>
       <c r="C6">
-        <v>29613</v>
+        <v>8094</v>
       </c>
       <c r="D6">
-        <v>24482</v>
+        <v>7221</v>
       </c>
       <c r="E6">
-        <v>20270</v>
+        <v>6514</v>
       </c>
       <c r="F6">
-        <v>106733</v>
+        <v>31182</v>
       </c>
       <c r="G6">
-        <v>115985</v>
+        <v>21909</v>
       </c>
       <c r="H6">
-        <v>122981</v>
+        <v>17958</v>
       </c>
       <c r="I6">
-        <v>127615</v>
+        <v>15035</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2186,28 +2186,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>16739</v>
+        <v>4332</v>
       </c>
       <c r="C7">
-        <v>14081</v>
+        <v>3819</v>
       </c>
       <c r="D7">
-        <v>11766</v>
+        <v>3411</v>
       </c>
       <c r="E7">
-        <v>9844</v>
+        <v>3082</v>
       </c>
       <c r="F7">
-        <v>49697</v>
+        <v>11680</v>
       </c>
       <c r="G7">
-        <v>53932</v>
+        <v>9049</v>
       </c>
       <c r="H7">
-        <v>56603</v>
+        <v>7436</v>
       </c>
       <c r="I7">
-        <v>57049</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2215,28 +2215,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>12269</v>
+        <v>2009</v>
       </c>
       <c r="C8">
-        <v>10516</v>
+        <v>1757</v>
       </c>
       <c r="D8">
-        <v>8857</v>
+        <v>1556</v>
       </c>
       <c r="E8">
-        <v>7412</v>
+        <v>1396</v>
       </c>
       <c r="F8">
-        <v>16399</v>
+        <v>4307</v>
       </c>
       <c r="G8">
-        <v>19082</v>
+        <v>2989</v>
       </c>
       <c r="H8">
-        <v>21291</v>
+        <v>2440</v>
       </c>
       <c r="I8">
-        <v>22896</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2244,28 +2244,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>11743187</v>
+        <v>1102993</v>
       </c>
       <c r="C9">
-        <v>11762910</v>
+        <v>870700</v>
       </c>
       <c r="D9">
-        <v>11375294</v>
+        <v>757691</v>
       </c>
       <c r="E9">
-        <v>10636200</v>
+        <v>667214</v>
       </c>
       <c r="F9">
-        <v>652929</v>
+        <v>656799</v>
       </c>
       <c r="G9">
-        <v>1070145</v>
+        <v>263535</v>
       </c>
       <c r="H9">
-        <v>1697006</v>
+        <v>210435</v>
       </c>
       <c r="I9">
-        <v>2529844</v>
+        <v>172729</v>
       </c>
     </row>
   </sheetData>
@@ -2332,28 +2332,28 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>646385</v>
+        <v>76755</v>
       </c>
       <c r="C4">
-        <v>667837</v>
+        <v>63046</v>
       </c>
       <c r="D4">
-        <v>668224</v>
+        <v>53049</v>
       </c>
       <c r="E4">
-        <v>654197</v>
+        <v>45087</v>
       </c>
       <c r="F4">
-        <v>30954</v>
+        <v>43564</v>
       </c>
       <c r="G4">
-        <v>46680</v>
+        <v>27354</v>
       </c>
       <c r="H4">
-        <v>66045</v>
+        <v>21060</v>
       </c>
       <c r="I4">
-        <v>85239</v>
+        <v>16590</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2361,28 +2361,28 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>583937</v>
+        <v>70280</v>
       </c>
       <c r="C5">
-        <v>585326</v>
+        <v>57950</v>
       </c>
       <c r="D5">
-        <v>571864</v>
+        <v>48451</v>
       </c>
       <c r="E5">
-        <v>550158</v>
+        <v>40879</v>
       </c>
       <c r="F5">
-        <v>63739</v>
+        <v>74641</v>
       </c>
       <c r="G5">
-        <v>88901</v>
+        <v>46290</v>
       </c>
       <c r="H5">
-        <v>116684</v>
+        <v>35402</v>
       </c>
       <c r="I5">
-        <v>142853</v>
+        <v>27662</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2390,28 +2390,28 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>301322</v>
+        <v>39951</v>
       </c>
       <c r="C6">
-        <v>289753</v>
+        <v>33789</v>
       </c>
       <c r="D6">
-        <v>276727</v>
+        <v>28881</v>
       </c>
       <c r="E6">
-        <v>263773</v>
+        <v>24935</v>
       </c>
       <c r="F6">
-        <v>228731</v>
+        <v>160553</v>
       </c>
       <c r="G6">
-        <v>252958</v>
+        <v>97392</v>
       </c>
       <c r="H6">
-        <v>273996</v>
+        <v>76259</v>
       </c>
       <c r="I6">
-        <v>291543</v>
+        <v>60997</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2419,28 +2419,28 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>134294</v>
+        <v>18692</v>
       </c>
       <c r="C7">
-        <v>129226</v>
+        <v>15777</v>
       </c>
       <c r="D7">
-        <v>123513</v>
+        <v>13467</v>
       </c>
       <c r="E7">
-        <v>117845</v>
+        <v>11620</v>
       </c>
       <c r="F7">
-        <v>106103</v>
+        <v>55280</v>
       </c>
       <c r="G7">
-        <v>117080</v>
+        <v>39371</v>
       </c>
       <c r="H7">
-        <v>126025</v>
+        <v>30839</v>
       </c>
       <c r="I7">
-        <v>132213</v>
+        <v>24661</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2448,28 +2448,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>72857</v>
+        <v>8978</v>
       </c>
       <c r="C8">
-        <v>70768</v>
+        <v>7535</v>
       </c>
       <c r="D8">
-        <v>67838</v>
+        <v>6395</v>
       </c>
       <c r="E8">
-        <v>64637</v>
+        <v>5486</v>
       </c>
       <c r="F8">
-        <v>29981</v>
+        <v>22304</v>
       </c>
       <c r="G8">
-        <v>35416</v>
+        <v>13208</v>
       </c>
       <c r="H8">
-        <v>40478</v>
+        <v>10272</v>
       </c>
       <c r="I8">
-        <v>44917</v>
+        <v>8173</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2477,28 +2477,28 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>41059046</v>
+        <v>5891822</v>
       </c>
       <c r="C9">
-        <v>43245310</v>
+        <v>4081402</v>
       </c>
       <c r="D9">
-        <v>44157268</v>
+        <v>3421600</v>
       </c>
       <c r="E9">
-        <v>44178249</v>
+        <v>2900653</v>
       </c>
       <c r="F9">
-        <v>814181</v>
+        <v>4195458</v>
       </c>
       <c r="G9">
-        <v>1262579</v>
+        <v>1234771</v>
       </c>
       <c r="H9">
-        <v>1937061</v>
+        <v>935359</v>
       </c>
       <c r="I9">
-        <v>2877706</v>
+        <v>734106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>